<commit_message>
Feat: Finish the UI of first screen
</commit_message>
<xml_diff>
--- a/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
+++ b/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5709" uniqueCount="122">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,246 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">result 的啦</t>
+  </si>
+  <si>
+    <t xml:space="preserve">result :p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sleepy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_txt_debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicked: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clicked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdefg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;result&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">" "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"+-*/. "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"+-*/."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTUST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bomb count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GenYoMinTW-Heavy.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTUST 林琨霖</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1624,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>103</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1404,13 +1646,13 @@
     </row>
     <row r="5" spans="2:16">
       <c r="B5" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1437,23 +1679,6 @@
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6"/>
-      <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
@@ -1600,6 +1825,454 @@
       <c r="F3" t="s">
         <v>36</v>
       </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Feat: Finish UI of screen_game
</commit_message>
<xml_diff>
--- a/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
+++ b/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5885" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7485" uniqueCount="137">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -384,6 +384,48 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bomb cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789 :APM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
   </si>
 </sst>
 </file>
@@ -1626,9 +1668,11 @@
         <v>17</v>
       </c>
       <c r="G4"/>
-      <c r="H4"/>
+      <c r="H4" t="s">
+        <v>128</v>
+      </c>
       <c r="I4" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
@@ -2294,6 +2338,125 @@
         <v>115</v>
       </c>
     </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
misc: UI: alignment, add background, color
</commit_message>
<xml_diff>
--- a/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
+++ b/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7485" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7704" uniqueCount="137">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2346,7 +2346,7 @@
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
misc: UI: Add TextArea as unclicked counts, function not implmented
This new TextArea displays the remaining non-bomb button to click
</commit_message>
<xml_diff>
--- a/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
+++ b/lab03_minesweeper/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7704" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8397" uniqueCount="140">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -426,6 +426,15 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unclick cnt</t>
   </si>
 </sst>
 </file>
@@ -2369,7 +2378,7 @@
         <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33">
@@ -2455,6 +2464,40 @@
       </c>
       <c r="F37" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>